<commit_message>
2.1.3: Clear column number on tableblock parse ending, for enabling multi sheet in a book which contains a table that has different number of columns
</commit_message>
<xml_diff>
--- a/test/calc/parser/t005/t005.xlsx
+++ b/test/calc/parser/t005/t005.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCommons/test/calc/parser/t005/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC034D6-FABD-9548-B2B6-BECD8B072050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA8183D-03E9-E246-A91D-877EDEC32858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11280" yWindow="1820" windowWidth="23840" windowHeight="18360" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="9" r:id="rId1"/>
-    <sheet name="config" sheetId="10" r:id="rId2"/>
+    <sheet name="コンフィグ" sheetId="10" r:id="rId2"/>
     <sheet name="readme" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="httpCode">config!$B$3:$B$4</definedName>
-    <definedName name="httpStatus">config!$B$3:$C$4</definedName>
+    <definedName name="httpCode">コンフィグ!$B$3:$B$4</definedName>
+    <definedName name="httpStatus">コンフィグ!$B$3:$C$4</definedName>
     <definedName name="Submit有無">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
@@ -2061,8 +2061,8 @@
   </sheetPr>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2316,7 +2316,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="28" t="str">
-        <f>INDEX(httpStatus, MATCH(config!F3, httpCode, 0), 2)</f>
+        <f>INDEX(httpStatus, MATCH(コンフィグ!F3, httpCode, 0), 2)</f>
         <v>CONTINUE</v>
       </c>
       <c r="D21" s="16"/>

</xml_diff>